<commit_message>
modificados:     formularios/form_calcimp_design.py actualizar tabla histutil(pendiente) 	modificados:     formularios/form_calculo_utilidades.py
</commit_message>
<xml_diff>
--- a/app-RRHH/file/list_invalidados.xlsx
+++ b/app-RRHH/file/list_invalidados.xlsx
@@ -151,7 +151,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -193,6 +193,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">

</xml_diff>